<commit_message>
Poprawiona tabela por roku i proba geom_smooth ale ich nie ma na wykresach
</commit_message>
<xml_diff>
--- a/Tabela_miesiace.xlsx
+++ b/Tabela_miesiace.xlsx
@@ -1,13 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zuzia\Documents\studia\Przetwarzanie danych środowiskowych\Białystok\Przetwarzanie_danych_srodowiskowych\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A240B2BA-A452-4296-A95A-2D4866D3B4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -17,66 +25,68 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t xml:space="preserve">I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">II</t>
-  </si>
-  <si>
-    <t xml:space="preserve">III</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VII</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VIII</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XII</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Średnia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mediana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Odchylenie Standardowe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Minimum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maximum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rozstęp miedzykwartylowy</t>
+    <t>I</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>VII</t>
+  </si>
+  <si>
+    <t>VIII</t>
+  </si>
+  <si>
+    <t>IX</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>XI</t>
+  </si>
+  <si>
+    <t>XII</t>
+  </si>
+  <si>
+    <t>Średnia</t>
+  </si>
+  <si>
+    <t>Mediana</t>
+  </si>
+  <si>
+    <t>Odchylenie Standardowe</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Rozstęp miedzykwartylowy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -84,16 +94,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF7C80"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC5C6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA7A9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -101,17 +145,316 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+      <color rgb="FFFFA7A9"/>
+      <color rgb="FFFFC5C6"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -393,302 +736,311 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="n">
-        <v>-3.64657534246575</v>
-      </c>
-      <c r="C2" t="n">
+      <c r="B2" s="17">
+        <v>-3.6465753424657499</v>
+      </c>
+      <c r="C2" s="18">
         <v>-2.9986301369863</v>
       </c>
-      <c r="D2" t="n">
-        <v>0.826027397260274</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="D2" s="18">
+        <v>0.82602739726027397</v>
+      </c>
+      <c r="E2" s="18">
         <v>7.13698630136986</v>
       </c>
-      <c r="F2" t="n">
-        <v>12.8068493150685</v>
-      </c>
-      <c r="G2" t="n">
-        <v>16.3767123287671</v>
-      </c>
-      <c r="H2" t="n">
-        <v>17.9178082191781</v>
-      </c>
-      <c r="I2" t="n">
+      <c r="F2" s="18">
+        <v>12.806849315068501</v>
+      </c>
+      <c r="G2" s="18">
+        <v>16.376712328767098</v>
+      </c>
+      <c r="H2" s="18">
+        <v>17.917808219178099</v>
+      </c>
+      <c r="I2" s="18">
         <v>17.0150684931507</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2" s="18">
         <v>12.3561643835616</v>
       </c>
-      <c r="K2" t="n">
-        <v>7.38356164383562</v>
-      </c>
-      <c r="L2" t="n">
-        <v>2.39452054794521</v>
-      </c>
-      <c r="M2" t="n">
+      <c r="K2" s="18">
+        <v>7.3835616438356197</v>
+      </c>
+      <c r="L2" s="18">
+        <v>2.3945205479452101</v>
+      </c>
+      <c r="M2" s="19">
         <v>-1.54931506849315</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="10">
         <v>-3.4</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3" s="5">
         <v>-2.6</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" s="5">
         <v>1.6</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" s="5">
         <v>7.2</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" s="5">
         <v>12.7</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" s="5">
         <v>16.2</v>
       </c>
-      <c r="H3" t="n">
-        <v>17.9</v>
-      </c>
-      <c r="I3" t="n">
-        <v>16.9</v>
-      </c>
-      <c r="J3" t="n">
+      <c r="H3" s="5">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="I3" s="5">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="J3" s="5">
         <v>12.3</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3" s="5">
         <v>7.5</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3" s="5">
         <v>2.5</v>
       </c>
-      <c r="M3" t="n">
+      <c r="M3" s="6">
         <v>-1.2</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="n">
-        <v>3.53907089940993</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="B4" s="9">
+        <v>3.5390708994099298</v>
+      </c>
+      <c r="C4" s="1">
         <v>3.74204686823657</v>
       </c>
-      <c r="D4" t="n">
-        <v>2.65920975089198</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="D4" s="1">
+        <v>2.6592097508919799</v>
+      </c>
+      <c r="E4" s="1">
         <v>1.60325249703663</v>
       </c>
-      <c r="F4" t="n">
-        <v>1.63242566336821</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="F4" s="1">
+        <v>1.6324256633682099</v>
+      </c>
+      <c r="G4" s="1">
         <v>1.53274631407748</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4" s="1">
         <v>1.6273992941836</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" s="1">
         <v>1.3882114024965</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J4" s="1">
         <v>1.45582987992052</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K4" s="1">
         <v>1.52187874559248</v>
       </c>
-      <c r="L4" t="n">
+      <c r="L4" s="1">
         <v>1.99853351867472</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M4" s="2">
         <v>2.66438044120284</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="10">
         <v>-15.1</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C5" s="5">
         <v>-13</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" s="5">
         <v>-6.1</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" s="5">
         <v>3.7</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5" s="5">
         <v>8.6</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" s="5">
         <v>13.7</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5" s="5">
         <v>13.9</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5" s="5">
         <v>14.2</v>
       </c>
-      <c r="J5" t="n">
-        <v>9.7</v>
-      </c>
-      <c r="K5" t="n">
+      <c r="J5" s="5">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="K5" s="5">
         <v>4</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L5" s="5">
         <v>-3.8</v>
       </c>
-      <c r="M5" t="n">
-        <v>-9.3</v>
+      <c r="M5" s="6">
+        <v>-9.3000000000000007</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="11">
         <v>2</v>
       </c>
-      <c r="C6" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="D6" t="n">
+      <c r="C6" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D6" s="3">
         <v>5.6</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="3">
         <v>11.7</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6" s="3">
         <v>16.7</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" s="3">
         <v>20.8</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6" s="3">
         <v>21.5</v>
       </c>
-      <c r="I6" t="n">
-        <v>20.1</v>
-      </c>
-      <c r="J6" t="n">
+      <c r="I6" s="3">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="J6" s="3">
         <v>16.8</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K6" s="3">
         <v>10.4</v>
       </c>
-      <c r="L6" t="n">
+      <c r="L6" s="3">
         <v>5.7</v>
       </c>
-      <c r="M6" t="n">
+      <c r="M6" s="4">
         <v>3.3</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="12">
         <v>3.7</v>
       </c>
-      <c r="C7" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="D7" t="n">
+      <c r="C7" s="7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="D7" s="7">
         <v>3.7</v>
       </c>
-      <c r="E7" t="n">
-        <v>2.3</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="E7" s="7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F7" s="7">
         <v>2.1</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" s="7">
         <v>2</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7" s="7">
         <v>1.8</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" s="7">
         <v>1.6</v>
       </c>
-      <c r="J7" t="n">
-        <v>2.2</v>
-      </c>
-      <c r="K7" t="n">
+      <c r="J7" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K7" s="7">
         <v>1.9</v>
       </c>
-      <c r="L7" t="n">
+      <c r="L7" s="7">
         <v>2.5</v>
       </c>
-      <c r="M7" t="n">
+      <c r="M7" s="8">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>